<commit_message>
[WIP] - Removing some redundant code from Match/Game, these share a lot right now, unnecessarily. - Looking at implementing singleton pattern for Dice and Log, I think this is appropriate. - Moving the burden for player/dice/log instantiation into the Game itself, see no need for these things to be passed around
</commit_message>
<xml_diff>
--- a/out/production/COMP41670_Group_Project/Test Strategy.xlsx
+++ b/out/production/COMP41670_Group_Project/Test Strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79738e9b9c1f34f3/MSc/41670 Software Engineering/Group_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{B813F0D1-8B60-4A61-9B7A-E5FE2B6792D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32264C06-995B-4FBA-93BB-BD780B974CE7}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{B813F0D1-8B60-4A61-9B7A-E5FE2B6792D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03CFCA12-0182-4B20-BF73-C5ECB4EBBBC2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC64A86E-5228-4C9F-A273-8C9B43EE2FC5}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D31" sqref="C28:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,37 +1308,37 @@
       <c r="B28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>